<commit_message>
2025-02-04 Se suben correcciones a budget.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/PlantillaCargaForecast.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/PlantillaCargaForecast.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\NuevoPortal\CódigoFuente\BitacorasProduccion\Content\plantillas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60E7B4E-B71F-47B8-B97D-85E76B7D136C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AD4CEC-849A-4D8E-B1D9-33EDE9E82DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94F15A3A-2C39-4D08-A181-F0A1CCA783E2}"/>
+    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15840" xr2:uid="{94F15A3A-2C39-4D08-A181-F0A1CCA783E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,20 @@
     <author>Xochitemol Cruz, Alfredo</author>
   </authors>
   <commentList>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{FCF32429-AE3B-4719-91EA-AF91E5D24D4C}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{D32B7186-F94A-4B08-980D-C722B3A6FAF5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Coloca una 'X' si deseas mostrar una advertencia al generar el reporte</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{FCF32429-AE3B-4719-91EA-AF91E5D24D4C}">
       <text>
         <r>
           <rPr>
@@ -65,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{9A32863F-1822-4FE3-B00B-F34A83563DE3}">
+    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{9A32863F-1822-4FE3-B00B-F34A83563DE3}">
       <text>
         <r>
           <rPr>
@@ -89,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{8C755CAF-01A7-4913-8B92-325303982B38}">
+    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{8C755CAF-01A7-4913-8B92-325303982B38}">
       <text>
         <r>
           <rPr>
@@ -118,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
   <si>
     <t>POS</t>
   </si>
@@ -177,9 +190,6 @@
     <t>Outgoing freight / PART [USD]</t>
   </si>
   <si>
-    <t>Trans Silao  - SLP</t>
-  </si>
-  <si>
     <t>Outgoing freight</t>
   </si>
   <si>
@@ -384,9 +394,6 @@
     <t>VAS / to</t>
   </si>
   <si>
-    <t>Fase 2</t>
-  </si>
-  <si>
     <t>Freights Income USD / PART</t>
   </si>
   <si>
@@ -403,12 +410,24 @@
   </si>
   <si>
     <t>Neopreno USD/Paq</t>
+  </si>
+  <si>
+    <t>Trans Silao  - SLP (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>MuestraAdvertencia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -525,7 +544,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1"/>
@@ -534,9 +553,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -560,9 +586,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -600,7 +626,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -706,7 +732,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -848,7 +874,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -856,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2163AC44-5709-410E-9A3F-F96E3439872B}">
-  <dimension ref="A1:BA3"/>
+  <dimension ref="A1:BB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,66 +911,67 @@
     <col min="19" max="19" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="57.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="28" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="19" customWidth="1"/>
-    <col min="50" max="50" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="24.44140625" customWidth="1"/>
-    <col min="53" max="53" width="19.77734375" customWidth="1"/>
+    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="28.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19" customWidth="1"/>
+    <col min="51" max="51" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="24.44140625" customWidth="1"/>
+    <col min="54" max="54" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>2</v>
@@ -982,104 +1009,107 @@
       <c r="U1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AP1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AY1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="AV1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AW1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AX1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="BB1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AZ1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="BA1" s="4" t="s">
-        <v>94</v>
-      </c>
     </row>
-    <row r="2" spans="1:53" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>0</v>
       </c>
@@ -1087,317 +1117,320 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
         <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
       </c>
       <c r="K2">
         <v>946</v>
       </c>
       <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
       </c>
       <c r="O2">
         <v>5190</v>
       </c>
       <c r="P2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="10">
+        <v>138110649</v>
+      </c>
+      <c r="X2" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V2">
-        <v>138110649</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>30</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>32</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2">
-        <v>0.75</v>
       </c>
       <c r="AB2">
         <v>0.75</v>
       </c>
-      <c r="AC2" t="s">
-        <v>46</v>
+      <c r="AC2">
+        <v>0.75</v>
       </c>
       <c r="AD2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF2" t="s">
         <v>34</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2">
+        <v>18.799829999999996</v>
+      </c>
+      <c r="AH2">
+        <v>18.520999999999997</v>
+      </c>
+      <c r="AI2">
+        <v>0.27882999999999925</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>35</v>
       </c>
-      <c r="AF2">
-        <v>18.799829999999996</v>
-      </c>
-      <c r="AG2">
-        <v>18.520999999999997</v>
-      </c>
-      <c r="AH2">
-        <v>0.27882999999999925</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="AK2">
+        <v>1.0126999999999999</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>45.32</v>
+      </c>
+      <c r="AN2">
+        <v>1.0126999999999999</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0.13212459053469996</v>
+      </c>
+      <c r="AQ2" s="8">
+        <v>45687</v>
+      </c>
+      <c r="AR2">
+        <v>53.867508376405539</v>
+      </c>
+      <c r="AS2">
+        <v>0.88057540946530011</v>
+      </c>
+      <c r="AT2">
+        <v>46.839541073791644</v>
+      </c>
+      <c r="AU2" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2">
-        <v>1.0126999999999999</v>
-      </c>
-      <c r="AK2">
+      <c r="AV2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW2">
         <v>0</v>
       </c>
-      <c r="AL2">
-        <v>45.32</v>
-      </c>
-      <c r="AM2">
-        <v>1.0126999999999999</v>
-      </c>
-      <c r="AN2">
+      <c r="AX2">
+        <v>3.4</v>
+      </c>
+      <c r="AY2">
         <v>0</v>
       </c>
-      <c r="AO2">
-        <v>0.13212459053469996</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AQ2">
-        <v>53.867508376405539</v>
-      </c>
-      <c r="AR2">
-        <v>0.88057540946530011</v>
-      </c>
-      <c r="AS2">
-        <v>46.839541073791644</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV2">
+      <c r="AZ2">
+        <v>0.24867470369746042</v>
+      </c>
+      <c r="BA2">
+        <v>2.8676589999999998E-2</v>
+      </c>
+      <c r="BB2">
         <v>0</v>
       </c>
-      <c r="AW2">
-        <v>3.4</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2">
-        <v>0.24867470369746042</v>
-      </c>
-      <c r="AZ2">
-        <v>2.8676589999999998E-2</v>
-      </c>
-      <c r="BA2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>60</v>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" t="s">
         <v>47</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>48</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
       </c>
       <c r="K3">
         <v>2021</v>
       </c>
       <c r="L3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
         <v>27</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
       </c>
       <c r="O3">
         <v>5190</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" t="s">
         <v>50</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>51</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>52</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="X3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y3" t="s">
         <v>53</v>
       </c>
-      <c r="U3" t="s">
-        <v>45</v>
-      </c>
-      <c r="V3" t="s">
-        <v>91</v>
-      </c>
-      <c r="W3" t="s">
-        <v>91</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>54</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>55</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA3">
-        <v>2</v>
       </c>
       <c r="AB3">
         <v>2</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE3" t="s">
         <v>57</v>
       </c>
-      <c r="AD3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF3">
+      <c r="AF3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG3">
         <v>10.809749999999999</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>9.15</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>1.6597499999999989</v>
       </c>
-      <c r="AI3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ3">
+      <c r="AJ3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK3">
         <v>0.21</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
       </c>
       <c r="AL3">
         <v>0</v>
       </c>
       <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
         <v>0.21</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>0</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>0.63273277420474705</v>
       </c>
-      <c r="AP3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AQ3">
+      <c r="AQ3" s="8">
+        <v>45955</v>
+      </c>
+      <c r="AR3">
         <v>19.426906265177269</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>-0.42273277420474709</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>-39.106618950923668</v>
       </c>
-      <c r="AT3" t="s">
-        <v>59</v>
-      </c>
       <c r="AU3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV3">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>37</v>
       </c>
       <c r="AW3">
         <v>0</v>
       </c>
       <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
         <v>24</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>0</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>1.3520329999999997E-2</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>0.65877301588224235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2025-02-05 Se completan mejoras a reporte de forecast.
</commit_message>
<xml_diff>
--- a/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/PlantillaCargaForecast.xlsx
+++ b/CódigoFuente/BitacorasProduccion/Content/plantillas_excel/PlantillaCargaForecast.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\NuevoPortal\CódigoFuente\BitacorasProduccion\Content\plantillas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AD4CEC-849A-4D8E-B1D9-33EDE9E82DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9BEC59-87CB-406A-B311-920CBD3382ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15840" xr2:uid="{94F15A3A-2C39-4D08-A181-F0A1CCA783E2}"/>
   </bookViews>
@@ -41,7 +41,33 @@
     <author>Xochitemol Cruz, Alfredo</author>
   </authors>
   <commentList>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{D32B7186-F94A-4B08-980D-C722B3A6FAF5}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{667346AB-77A0-4E5E-8E2A-2654FAD0D010}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>La celda debe ser de tipo texto y seguir el formato YYYY-MM, ejemplo 2024-05. Vacío = muestra todo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{EAEB3A10-486F-411A-B406-68C72B0DE3A9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>La celda debe ser de tipo texto y seguir el formato YYYY-MM, ejemplo 2024-05. Vacío = muestra todo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{D32B7186-F94A-4B08-980D-C722B3A6FAF5}">
       <text>
         <r>
           <rPr>
@@ -54,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{FCF32429-AE3B-4719-91EA-AF91E5D24D4C}">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{FCF32429-AE3B-4719-91EA-AF91E5D24D4C}">
       <text>
         <r>
           <rPr>
@@ -78,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{9A32863F-1822-4FE3-B00B-F34A83563DE3}">
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{9A32863F-1822-4FE3-B00B-F34A83563DE3}">
       <text>
         <r>
           <rPr>
@@ -102,7 +128,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{8C755CAF-01A7-4913-8B92-325303982B38}">
+    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{E250CDBD-BCB6-44D5-BF68-676F85DA6676}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>La celda debe ser de tipo texto y seguir el formato YYYY-MM, ejemplo 2024-05</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{8C755CAF-01A7-4913-8B92-325303982B38}">
       <text>
         <r>
           <rPr>
@@ -131,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="102">
   <si>
     <t>POS</t>
   </si>
@@ -412,22 +451,37 @@
     <t>Neopreno USD/Paq</t>
   </si>
   <si>
-    <t>Trans Silao  - SLP (YYYY-MM-DD)</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>MuestraAdvertencia</t>
+  </si>
+  <si>
+    <t>2025-12</t>
+  </si>
+  <si>
+    <t>Trans Silao  - SLP (YYYY-MM)</t>
+  </si>
+  <si>
+    <t>Inicio Demanda(YYYY-MM)</t>
+  </si>
+  <si>
+    <t>Fin Demanda(YYYY-MM)</t>
+  </si>
+  <si>
+    <t>2024-12</t>
+  </si>
+  <si>
+    <t>2025-05</t>
+  </si>
+  <si>
+    <t>2025-10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -544,7 +598,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1"/>
@@ -556,13 +610,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -583,6 +644,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -882,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2163AC44-5709-410E-9A3F-F96E3439872B}">
-  <dimension ref="A1:BB3"/>
+  <dimension ref="A1:BD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,41 +976,43 @@
     <col min="19" max="19" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="57.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="28" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="28.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19" customWidth="1"/>
-    <col min="51" max="51" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="52" max="53" width="24.44140625" customWidth="1"/>
-    <col min="54" max="54" width="19.77734375" customWidth="1"/>
+    <col min="22" max="22" width="27.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="28" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="28.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19" customWidth="1"/>
+    <col min="53" max="53" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="24.44140625" customWidth="1"/>
+    <col min="56" max="56" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:56" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
@@ -1009,107 +1076,113 @@
       <c r="U1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>95</v>
+      <c r="V1" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="W1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AQ1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>0</v>
       </c>
@@ -1173,104 +1246,104 @@
       <c r="U2" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="10">
+      <c r="Y2" s="8">
         <v>138110649</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>31</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>32</v>
       </c>
-      <c r="AB2">
+      <c r="AD2">
         <v>0.75</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>0.75</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>45</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>34</v>
       </c>
-      <c r="AG2">
+      <c r="AI2">
         <v>18.799829999999996</v>
       </c>
-      <c r="AH2">
+      <c r="AJ2">
         <v>18.520999999999997</v>
       </c>
-      <c r="AI2">
+      <c r="AK2">
         <v>0.27882999999999925</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>35</v>
       </c>
-      <c r="AK2">
+      <c r="AM2">
         <v>1.0126999999999999</v>
       </c>
-      <c r="AL2">
+      <c r="AN2">
         <v>0</v>
       </c>
-      <c r="AM2">
+      <c r="AO2">
         <v>45.32</v>
       </c>
-      <c r="AN2">
+      <c r="AP2">
         <v>1.0126999999999999</v>
       </c>
-      <c r="AO2">
+      <c r="AQ2">
         <v>0</v>
       </c>
-      <c r="AP2">
+      <c r="AR2">
         <v>0.13212459053469996</v>
       </c>
-      <c r="AQ2" s="8">
-        <v>45687</v>
-      </c>
-      <c r="AR2">
+      <c r="AS2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT2">
         <v>53.867508376405539</v>
       </c>
-      <c r="AS2">
+      <c r="AU2">
         <v>0.88057540946530011</v>
       </c>
-      <c r="AT2">
+      <c r="AV2">
         <v>46.839541073791644</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AW2" t="s">
         <v>36</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AX2" t="s">
         <v>37</v>
-      </c>
-      <c r="AW2">
-        <v>0</v>
-      </c>
-      <c r="AX2">
-        <v>3.4</v>
       </c>
       <c r="AY2">
         <v>0</v>
       </c>
       <c r="AZ2">
+        <v>3.4</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
         <v>0.24867470369746042</v>
       </c>
-      <c r="BA2">
+      <c r="BC2">
         <v>2.8676589999999998E-2</v>
       </c>
-      <c r="BB2">
+      <c r="BD2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>59</v>
       </c>
@@ -1334,103 +1407,109 @@
       <c r="U3" t="s">
         <v>44</v>
       </c>
-      <c r="V3" t="s">
-        <v>94</v>
+      <c r="V3" s="10" t="s">
+        <v>101</v>
       </c>
       <c r="W3" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="X3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>89</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>53</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>54</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
         <v>55</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>2</v>
       </c>
-      <c r="AC3">
+      <c r="AE3">
         <v>2</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AF3" t="s">
         <v>56</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>57</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AH3" t="s">
         <v>34</v>
       </c>
-      <c r="AG3">
+      <c r="AI3">
         <v>10.809749999999999</v>
       </c>
-      <c r="AH3">
+      <c r="AJ3">
         <v>9.15</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>1.6597499999999989</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AL3" t="s">
         <v>28</v>
       </c>
-      <c r="AK3">
+      <c r="AM3">
         <v>0.21</v>
       </c>
-      <c r="AL3">
+      <c r="AN3">
         <v>0</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0.21</v>
       </c>
       <c r="AO3">
         <v>0</v>
       </c>
       <c r="AP3">
+        <v>0.21</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
         <v>0.63273277420474705</v>
       </c>
-      <c r="AQ3" s="8">
-        <v>45955</v>
-      </c>
-      <c r="AR3">
+      <c r="AS3" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AT3">
         <v>19.426906265177269</v>
       </c>
-      <c r="AS3">
+      <c r="AU3">
         <v>-0.42273277420474709</v>
       </c>
-      <c r="AT3">
+      <c r="AV3">
         <v>-39.106618950923668</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AW3" t="s">
         <v>58</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AX3" t="s">
         <v>37</v>
       </c>
-      <c r="AW3">
+      <c r="AY3">
         <v>0</v>
-      </c>
-      <c r="AX3">
-        <v>0</v>
-      </c>
-      <c r="AY3">
-        <v>24</v>
       </c>
       <c r="AZ3">
         <v>0</v>
       </c>
       <c r="BA3">
+        <v>24</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
         <v>1.3520329999999997E-2</v>
       </c>
-      <c r="BB3">
+      <c r="BD3">
         <v>0.65877301588224235</v>
       </c>
     </row>

</xml_diff>